<commit_message>
successful integration of dynamodb
</commit_message>
<xml_diff>
--- a/weekly_financial_report_2023-08-01_to_2023-08-07.xlsx
+++ b/weekly_financial_report_2023-08-01_to_2023-08-07.xlsx
@@ -448,7 +448,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Komponen</t>
+          <t>Component</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -458,53 +458,59 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Jumlah</t>
+          <t>Amount</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Jasa 101</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>101</v>
+          <t>Service 102</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>102</t>
+        </is>
       </c>
       <c r="C2" s="2" t="n">
-        <v>32562.72</v>
+        <v>218.88</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Jasa 102</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>102</v>
+          <t>Service 103</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>103</t>
+        </is>
       </c>
       <c r="C3" s="2" t="n">
-        <v>11727.88</v>
+        <v>713.6999999999999</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Jasa 103</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>103</v>
+          <t>Service 101</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>101</t>
+        </is>
       </c>
       <c r="C4" s="2" t="n">
-        <v>6583.2</v>
+        <v>2144.84</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Total Pendapatan</t>
+          <t>Total Sales</t>
         </is>
       </c>
       <c r="C5" s="2" t="n">
@@ -514,7 +520,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Laba Rugi Harian</t>
+          <t>Daily Profit and Loss</t>
         </is>
       </c>
       <c r="B6" s="2" t="n">
@@ -524,7 +530,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Total Arus Kas</t>
+          <t>Total Cash Flow</t>
         </is>
       </c>
       <c r="B7" s="2" t="n">
@@ -534,7 +540,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Saldo Kas Harian</t>
+          <t>Daily Cash Balance</t>
         </is>
       </c>
       <c r="B8" s="2" t="n">
@@ -544,31 +550,31 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Total Aset</t>
+          <t>Total Assets</t>
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>40000000</v>
+        <v>10093.75999999999</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Total Utang</t>
+          <t>Total Debt</t>
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>8000000</v>
+        <v>800000</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Total Ekuitas</t>
+          <t>Total Equity</t>
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>32000000</v>
+        <v>-789906.24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>